<commit_message>
Upload of some documentation
</commit_message>
<xml_diff>
--- a/Documentation/RiskAssessmentQAProject1.xlsx
+++ b/Documentation/RiskAssessmentQAProject1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harpr\Desktop\QA\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harpr\Desktop\QA\Projects\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61960698-CF94-4B85-AC9F-1C5053E814A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073F644D-8245-4B7B-BD78-B6DAB45FE86D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="446" windowWidth="13680" windowHeight="14983" xr2:uid="{D70316BA-2B41-4A2E-9786-400113271AB7}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15634" xr2:uid="{D70316BA-2B41-4A2E-9786-400113271AB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>RISK</t>
   </si>
@@ -54,9 +54,6 @@
     <t>PROPOSED MEASURES</t>
   </si>
   <si>
-    <t>RESPONSE</t>
-  </si>
-  <si>
     <t>Database can be attacked via SQL Injection and could lead to a breach of user data including email's and password</t>
   </si>
   <si>
@@ -73,6 +70,45 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>While testing is being conducted alongside the development, the current testing is just smoke testing which check the basic functionality of the application. While certain methods implemented in the code contain some sort of validation by making sure the correct data is inserted, this needs to be tested at a lower level</t>
+  </si>
+  <si>
+    <t>The database can be accessed if the adminstrators account were to be hacked. This would mean that whoever had accessed the account, they could modify any data or even delete the database.</t>
+  </si>
+  <si>
+    <t>One solution that is not in place is to credit the account so that on the off chance that the account was to lose all its credit, the service could still run. While this is a viable option, given the amount of credit that is available, it seems highly unlikely that it would run out. Another solution is to create a new Google account. If the application is constantly being saved and uploaded to a version control system, the project can be cloned to this new account and can resume its operations.</t>
+  </si>
+  <si>
+    <t>The virtual machine and SQL instance are both being shut down while not in use to reduce costs. Also, to limit the usage of the virutal machine, the application is being developed outside it so the machine can be turned off until the application needs to be tested. Finally, as the application is a basic application, it does not need huge amounts of processing power or a high storage capacity so the choices for both storage size and performance of the virtual machine have both been taken into consideration and have suitable hardware for its requirements</t>
+  </si>
+  <si>
+    <t>The database can only be accessed by a single Google account which has a secure password and is also secured with two factor authenication. This means that even if the the password was comprimised, there would still be another layer of authentication required to access the account. Furthermore, the database itself can be created with a password which in this case, it has, increasing the security on the database and reducing the chance of someone getting unauthorised access.</t>
+  </si>
+  <si>
+    <t>Thourough tests to be conducted and in doing these tests, any flaws in the application which can lead to a potential bug or provide a way for unauthorised users can be found while testing and couldn be fixed before launching the application</t>
+  </si>
+  <si>
+    <t>As user data can be comprimised, the impact of this is high. One of the measures in place is validation. This means that certain fields have to match a certain criteria to access the application. For example, the email has to be in the email format and pages where a ID is required compared to text, are checked and will give an error stating that an ID is required.</t>
+  </si>
+  <si>
+    <t>Research into proposed measures suggest that queries should be split up and should contain placeholders for parameters. Once the parameters have been validated, they should then be passed through to the split query.. Once all the parameters have been validated, the query is then binded together and then executed</t>
+  </si>
+  <si>
+    <t>The measures in place should already be enough to prevent any unauthorised access but further security can be implemented by perhaps using different methods of authentication such as a security key.</t>
+  </si>
+  <si>
+    <t>Testing could reveal faults in the program. Testing is a very important part in developing the application and running tests late in the development could raise issues and bugs which has previously not been seen.</t>
+  </si>
+  <si>
+    <t>Upload of any keys or certain passwords required to access upload to a VCS. Uploading these keys will allow anyone with access to the repository to view these keys and allow them to gain unauthorised access</t>
+  </si>
+  <si>
+    <t>Any keys have been exported as an environment variable meaning that they have to be imported each time a new bash shell is opened. This means that anyone who tries to launch the application without the keys will fail. Having this means that only people with access to these keys will be able to launch the application.</t>
+  </si>
+  <si>
+    <t>The measures in place should already be enough to prevent this risk from occuring. One measure that could be implemented is to prevent excessive sharing of the keys and keep it between a select few and potentially change the password or data for the key on a regular basis such that if a key was uploaded, an updated key would render it obsolete.</t>
   </si>
 </sst>
 </file>
@@ -120,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -171,44 +207,153 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,240 +669,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9B7BBA-5194-4C0E-A45C-48B8E683C59F}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="B1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="92" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="7.3046875" customWidth="1"/>
-    <col min="5" max="5" width="7.765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.765625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="6" width="7.765625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.765625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="18.765625" style="17" customWidth="1"/>
+    <col min="11" max="13" width="16.07421875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="2:19" ht="15.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="2:19" ht="15.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="2:19" ht="91.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" spans="1:15" ht="60.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="12" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11" t="s">
+      <c r="F4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="2:19" ht="116.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="G5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="H5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="2:19" s="2" customFormat="1" ht="133.30000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-    </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" ht="100.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="10" t="s">
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+    </row>
+    <row r="7" spans="2:19" ht="91.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.4">
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.4">
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.4">
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.4">
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="2:19" ht="101.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="G11" s="30"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="G12" s="30"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="G13" s="30"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="G14" s="30"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="G15" s="30"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="G16" s="30"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.4">
+      <c r="G17" s="30"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.4">
+      <c r="G18" s="30"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.4">
+      <c r="G19" s="30"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.4">
+      <c r="G20" s="30"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.4">
+      <c r="G21" s="30"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="M2:O3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I3"/>
-    <mergeCell ref="J2:L3"/>
+  <mergeCells count="22">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="K2:M3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>